<commit_message>
Test data from invalid login page
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B126 7PM Selenium\share\Day25-10-04-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B126 7PM Selenium\workspace\B126AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305AF204-4DCF-480F-A484-A4AA01EF2F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FBCB68-8BAD-41DA-B777-EDEB6B77228F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="script1" sheetId="1" r:id="rId1"/>
+    <sheet name="valid_login" sheetId="2" r:id="rId2"/>
+    <sheet name="invalid_login" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +27,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>akshara</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pointofsale</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -350,7 +367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -369,4 +386,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8D3F12-2F03-41EC-B295-E4C969D797DE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF208D2-F997-4D54-B3E1-99472B92EAF3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>